<commit_message>
added labels for functional tables
</commit_message>
<xml_diff>
--- a/adapter/tests/test_w_inputs_from_files_table.xlsx
+++ b/adapter/tests/test_w_inputs_from_files_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22152"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="14208"/>
   </bookViews>
   <sheets>
     <sheet name="test - Copy" sheetId="1" r:id="rId1"/>
@@ -18,48 +18,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>mgrahovac</author>
-  </authors>
-  <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>mgrahovac:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value ensures that each run with identical inputs produces identical outputs</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Sample Size</t>
-  </si>
-  <si>
-    <t>Seed Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Output Path</t>
   </si>
@@ -107,13 +67,34 @@
   </si>
   <si>
     <t>cc</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>Query Only</t>
+  </si>
+  <si>
+    <t>\adapter\tests\test.db</t>
+  </si>
+  <si>
+    <t>table1, table2, table3</t>
+  </si>
+  <si>
+    <t>N, Y, N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\adapter\tests\test.xlsx		</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,19 +228,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -689,15 +657,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="run_parameters7" displayName="run_parameters7" ref="B2:E3" totalsRowShown="0">
-  <autoFilter ref="B2:E3"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Sample Size"/>
-    <tableColumn id="2" name="Seed Value"/>
-    <tableColumn id="3" name="Output Path"/>
-    <tableColumn id="4" name="Version"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="run_parameters7" displayName="run_parameters7" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Output Path"/>
+    <tableColumn id="2" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="inputs_from_files" displayName="inputs_from_files" ref="B7:D9" totalsRowShown="0">
+  <autoFilter ref="B7:D9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="File Path"/>
+    <tableColumn id="2" name="Table Name"/>
+    <tableColumn id="3" name="Query Only"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -963,14 +941,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -979,40 +962,28 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>165798</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L3">
         <v>12</v>
@@ -1023,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L4">
         <v>13</v>
@@ -1034,21 +1005,46 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L5">
         <v>45</v>
       </c>
     </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
       <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" t="s">
         <v>12</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -1056,7 +1052,7 @@
         <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L10">
         <v>112</v>
@@ -1067,7 +1063,7 @@
         <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L11">
         <v>113</v>
@@ -1078,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="K12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L12">
         <v>145</v>
@@ -1086,8 +1082,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>

</xml_diff>

<commit_message>
updated number of tables in the test
</commit_message>
<xml_diff>
--- a/adapter/tests/test_w_inputs_from_files_table.xlsx
+++ b/adapter/tests/test_w_inputs_from_files_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/mgrahovac/repos/adapter/adapter/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC4B046-5FBA-E441-A828-E7935032DF84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C144FB-98E7-4B41-91BC-9081ACD3D32F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57460" yWindow="2060" windowWidth="28780" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38460" yWindow="-3640" windowWidth="28780" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test - Copy" sheetId="1" r:id="rId1"/>
@@ -949,7 +949,7 @@
   <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Excel class, test files and adapter.i_o
</commit_message>
<xml_diff>
--- a/adapter/tests/test_w_inputs_from_files_table.xlsx
+++ b/adapter/tests/test_w_inputs_from_files_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/mgrahovac/repos/adapter/adapter/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rlan/Desktop/LBNL/ees/adapter/adapter/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C144FB-98E7-4B41-91BC-9081ACD3D32F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455B5340-0F70-D845-B624-6193BDE2D5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38460" yWindow="-3640" windowWidth="28780" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test - Copy" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Output Path</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>adapter/tests/test1.xlsx</t>
+  </si>
+  <si>
+    <t>xlsx_table1_in_other_excel_file</t>
   </si>
 </sst>
 </file>
@@ -949,7 +952,7 @@
   <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1041,6 +1044,9 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
       <c r="J9" t="s">
         <v>10</v>
       </c>

</xml_diff>